<commit_message>
added data model imports
</commit_message>
<xml_diff>
--- a/VerificationTemplate_Populated.xlsx
+++ b/VerificationTemplate_Populated.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26415"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sambhav/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sambhav/Desktop/pepConsulting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="87" documentId="8_{3A3FC7F3-ADA2-E543-A3C5-5770F3D6F748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C1D3E5DA-3DD6-4425-A788-6E3D13B57668}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E67E298-21CE-9745-A9E3-37D3FA85AA11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{5D1F851E-5631-2C4E-ACBB-76C0E1385F3F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="20260" xr2:uid="{5D1F851E-5631-2C4E-ACBB-76C0E1385F3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="170">
   <si>
     <t xml:space="preserve">Date of ERCP </t>
   </si>
@@ -540,13 +540,19 @@
   </si>
   <si>
     <t>MRN:  JH16121937</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>MRN:  JH16121935</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -559,6 +565,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -900,44 +907,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F7DFEBA-E98D-C74B-BBEA-B3F416C105BF}">
-  <dimension ref="A1:AB136"/>
+  <dimension ref="A1:AB138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="A110" workbookViewId="0">
+      <selection activeCell="D145" sqref="D145"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.75" customWidth="1"/>
-    <col min="4" max="4" width="14.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="26" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.25" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.75" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="42.625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="42.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.6640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="26.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.25" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="26.75" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21.375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="37.25" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="39.25" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="21.625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.75" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="37.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="39.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="20.625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="30.875" customWidth="1"/>
-    <col min="27" max="27" width="27.375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="31.875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="30.83203125" customWidth="1"/>
+    <col min="27" max="27" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="31.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="3" customFormat="1">
+    <row r="1" spans="1:28" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1023,7 +1030,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:28">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>44832</v>
       </c>
@@ -1109,7 +1116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:28">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>44832</v>
       </c>
@@ -1195,7 +1202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:28">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>44832</v>
       </c>
@@ -1281,7 +1288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:28">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>44830</v>
       </c>
@@ -1367,7 +1374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:28">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>44830</v>
       </c>
@@ -1453,7 +1460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:28">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>44830</v>
       </c>
@@ -1539,7 +1546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:28">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>44831</v>
       </c>
@@ -1625,7 +1632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:28">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>44831</v>
       </c>
@@ -1711,7 +1718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:28">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>44831</v>
       </c>
@@ -1797,7 +1804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:28">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>44831</v>
       </c>
@@ -1883,7 +1890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:28">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>44823</v>
       </c>
@@ -1969,7 +1976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:28">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>44823</v>
       </c>
@@ -2055,7 +2062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:28">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>44823</v>
       </c>
@@ -2141,7 +2148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:28">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>44824</v>
       </c>
@@ -2227,7 +2234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:28">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>44824</v>
       </c>
@@ -2313,7 +2320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:28">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>44824</v>
       </c>
@@ -2399,7 +2406,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:28">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>44824</v>
       </c>
@@ -2485,7 +2492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:28">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>44824</v>
       </c>
@@ -2571,7 +2578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:28">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>44824</v>
       </c>
@@ -2657,7 +2664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:28">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>44825</v>
       </c>
@@ -2743,7 +2750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:28">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>44825</v>
       </c>
@@ -2829,7 +2836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:28">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>44825</v>
       </c>
@@ -2915,7 +2922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:28">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>44825</v>
       </c>
@@ -3001,7 +3008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:28">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>44825</v>
       </c>
@@ -3087,7 +3094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:28">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>44825</v>
       </c>
@@ -3173,7 +3180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:28">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>44825</v>
       </c>
@@ -3259,7 +3266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:28">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>44825</v>
       </c>
@@ -3345,7 +3352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:28">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>44825</v>
       </c>
@@ -3431,7 +3438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:28">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>44825</v>
       </c>
@@ -3517,7 +3524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:28">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>44825</v>
       </c>
@@ -3603,7 +3610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:28">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>44825</v>
       </c>
@@ -3689,7 +3696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:28">
+    <row r="33" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>44826</v>
       </c>
@@ -3775,7 +3782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:28">
+    <row r="34" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>44826</v>
       </c>
@@ -3861,7 +3868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:28">
+    <row r="35" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>44827</v>
       </c>
@@ -3947,7 +3954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:28">
+    <row r="36" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>44827</v>
       </c>
@@ -4033,7 +4040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:28">
+    <row r="37" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>44827</v>
       </c>
@@ -4119,7 +4126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:28">
+    <row r="38" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>44827</v>
       </c>
@@ -4205,7 +4212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:28">
+    <row r="39" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>44816</v>
       </c>
@@ -4291,7 +4298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:28">
+    <row r="40" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>44816</v>
       </c>
@@ -4377,7 +4384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:28">
+    <row r="41" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>44817</v>
       </c>
@@ -4463,7 +4470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:28">
+    <row r="42" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>44817</v>
       </c>
@@ -4549,7 +4556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:28">
+    <row r="43" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>44817</v>
       </c>
@@ -4635,7 +4642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:28">
+    <row r="44" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>44818</v>
       </c>
@@ -4721,7 +4728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:28">
+    <row r="45" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>44818</v>
       </c>
@@ -4807,7 +4814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:28">
+    <row r="46" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>44818</v>
       </c>
@@ -4893,7 +4900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:28">
+    <row r="47" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>44819</v>
       </c>
@@ -4979,7 +4986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:28">
+    <row r="48" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>44820</v>
       </c>
@@ -5065,7 +5072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:28">
+    <row r="49" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>44820</v>
       </c>
@@ -5151,7 +5158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:28">
+    <row r="50" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>44820</v>
       </c>
@@ -5237,7 +5244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:28">
+    <row r="51" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>44820</v>
       </c>
@@ -5323,7 +5330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:28">
+    <row r="52" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>44810</v>
       </c>
@@ -5409,7 +5416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:28">
+    <row r="53" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>44810</v>
       </c>
@@ -5495,7 +5502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:28">
+    <row r="54" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>44810</v>
       </c>
@@ -5581,7 +5588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:28">
+    <row r="55" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>44810</v>
       </c>
@@ -5667,7 +5674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:28">
+    <row r="56" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>44810</v>
       </c>
@@ -5753,7 +5760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:28">
+    <row r="57" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>44810</v>
       </c>
@@ -5839,7 +5846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:28">
+    <row r="58" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>44810</v>
       </c>
@@ -5925,7 +5932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:28">
+    <row r="59" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>44810</v>
       </c>
@@ -6011,7 +6018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:28">
+    <row r="60" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>44810</v>
       </c>
@@ -6097,7 +6104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:28">
+    <row r="61" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>44811</v>
       </c>
@@ -6183,7 +6190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:28">
+    <row r="62" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>44811</v>
       </c>
@@ -6269,7 +6276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:28">
+    <row r="63" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>44811</v>
       </c>
@@ -6355,7 +6362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:28">
+    <row r="64" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>44811</v>
       </c>
@@ -6441,7 +6448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:28">
+    <row r="65" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>44811</v>
       </c>
@@ -6527,7 +6534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:28">
+    <row r="66" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>44811</v>
       </c>
@@ -6613,7 +6620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:28">
+    <row r="67" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>44813</v>
       </c>
@@ -6699,7 +6706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:28">
+    <row r="68" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>44813</v>
       </c>
@@ -6785,7 +6792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:28">
+    <row r="69" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>44813</v>
       </c>
@@ -6871,7 +6878,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:28">
+    <row r="70" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>44813</v>
       </c>
@@ -6957,7 +6964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:28">
+    <row r="71" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>44813</v>
       </c>
@@ -7043,7 +7050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:28">
+    <row r="72" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>44813</v>
       </c>
@@ -7129,7 +7136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:28">
+    <row r="73" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>44813</v>
       </c>
@@ -7215,7 +7222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:28">
+    <row r="74" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>44813</v>
       </c>
@@ -7301,7 +7308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:28">
+    <row r="75" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>44833</v>
       </c>
@@ -7387,7 +7394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:28">
+    <row r="76" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>44833</v>
       </c>
@@ -7473,7 +7480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:28">
+    <row r="77" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>44837</v>
       </c>
@@ -7559,7 +7566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:28">
+    <row r="78" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>44837</v>
       </c>
@@ -7645,7 +7652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:28">
+    <row r="79" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>44837</v>
       </c>
@@ -7731,7 +7738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:28">
+    <row r="80" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>44837</v>
       </c>
@@ -7817,7 +7824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:28">
+    <row r="81" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>44838</v>
       </c>
@@ -7903,7 +7910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:28">
+    <row r="82" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>44838</v>
       </c>
@@ -7989,7 +7996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:28">
+    <row r="83" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>44838</v>
       </c>
@@ -8075,7 +8082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:28">
+    <row r="84" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>44838</v>
       </c>
@@ -8161,7 +8168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:28">
+    <row r="85" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>44839</v>
       </c>
@@ -8247,7 +8254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:28">
+    <row r="86" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>44839</v>
       </c>
@@ -8333,7 +8340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:28">
+    <row r="87" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>44839</v>
       </c>
@@ -8419,7 +8426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:28">
+    <row r="88" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>44839</v>
       </c>
@@ -8505,7 +8512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:28">
+    <row r="89" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>44839</v>
       </c>
@@ -8591,7 +8598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:28">
+    <row r="90" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>44840</v>
       </c>
@@ -8677,7 +8684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:28">
+    <row r="91" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>44841</v>
       </c>
@@ -8763,7 +8770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:28">
+    <row r="92" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>44840</v>
       </c>
@@ -8849,7 +8856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:28">
+    <row r="93" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>44841</v>
       </c>
@@ -8935,7 +8942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:28">
+    <row r="94" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>44841</v>
       </c>
@@ -9021,7 +9028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:28">
+    <row r="95" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>44841</v>
       </c>
@@ -9107,7 +9114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:28">
+    <row r="96" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>44841</v>
       </c>
@@ -9190,7 +9197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:28">
+    <row r="97" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>44841</v>
       </c>
@@ -9276,7 +9283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:28">
+    <row r="98" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>44844</v>
       </c>
@@ -9362,7 +9369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:28">
+    <row r="99" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>44845</v>
       </c>
@@ -9448,7 +9455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:28">
+    <row r="100" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>44845</v>
       </c>
@@ -9534,7 +9541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:28">
+    <row r="101" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>44845</v>
       </c>
@@ -9620,7 +9627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:28">
+    <row r="102" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>44845</v>
       </c>
@@ -9706,7 +9713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:28">
+    <row r="103" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <v>44845</v>
       </c>
@@ -9792,7 +9799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:28">
+    <row r="104" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
         <v>44846</v>
       </c>
@@ -9878,7 +9885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:28">
+    <row r="105" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
         <v>44847</v>
       </c>
@@ -9964,7 +9971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:28">
+    <row r="106" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
         <v>44847</v>
       </c>
@@ -10050,7 +10057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:28">
+    <row r="107" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
         <v>44847</v>
       </c>
@@ -10136,7 +10143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:28">
+    <row r="108" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
         <v>44847</v>
       </c>
@@ -10222,7 +10229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:28">
+    <row r="109" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
         <v>44847</v>
       </c>
@@ -10308,7 +10315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:28">
+    <row r="110" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
         <v>44848</v>
       </c>
@@ -10394,7 +10401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:28">
+    <row r="111" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
         <v>44848</v>
       </c>
@@ -10480,7 +10487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:28">
+    <row r="112" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
         <v>44848</v>
       </c>
@@ -10566,7 +10573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:28">
+    <row r="113" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
         <v>44852</v>
       </c>
@@ -10652,7 +10659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:28">
+    <row r="114" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
         <v>44852</v>
       </c>
@@ -10738,7 +10745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:28">
+    <row r="115" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
         <v>44852</v>
       </c>
@@ -10824,7 +10831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:28">
+    <row r="116" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
         <v>44853</v>
       </c>
@@ -10910,7 +10917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:28">
+    <row r="117" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A117" s="1">
         <v>44853</v>
       </c>
@@ -10996,7 +11003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:28">
+    <row r="118" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
         <v>44853</v>
       </c>
@@ -11082,7 +11089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:28">
+    <row r="119" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A119" s="1">
         <v>44853</v>
       </c>
@@ -11168,7 +11175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:28">
+    <row r="120" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A120" s="1">
         <v>44858</v>
       </c>
@@ -11254,7 +11261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:28">
+    <row r="121" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
         <v>44858</v>
       </c>
@@ -11340,7 +11347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:28">
+    <row r="122" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A122" s="1">
         <v>44859</v>
       </c>
@@ -11426,7 +11433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:28">
+    <row r="123" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A123" s="1">
         <v>44860</v>
       </c>
@@ -11512,7 +11519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:28">
+    <row r="124" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A124" s="1">
         <v>44860</v>
       </c>
@@ -11598,7 +11605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:28">
+    <row r="125" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A125" s="1">
         <v>44861</v>
       </c>
@@ -11684,7 +11691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:28">
+    <row r="126" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A126" s="1">
         <v>44862</v>
       </c>
@@ -11770,7 +11777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:28">
+    <row r="127" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A127" s="1">
         <v>44862</v>
       </c>
@@ -11856,7 +11863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:28">
+    <row r="128" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A128" s="1">
         <v>44862</v>
       </c>
@@ -11942,7 +11949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:28">
+    <row r="129" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A129" s="1">
         <v>44862</v>
       </c>
@@ -12028,7 +12035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:28">
+    <row r="130" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A130" s="1">
         <v>44862</v>
       </c>
@@ -12114,7 +12121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:28">
+    <row r="131" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A131" s="1">
         <v>44862</v>
       </c>
@@ -12200,7 +12207,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:28">
+    <row r="132" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A132" s="1">
         <v>44862</v>
       </c>
@@ -12286,7 +12293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:28">
+    <row r="133" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A133" s="1">
         <v>44865</v>
       </c>
@@ -12372,7 +12379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:28">
+    <row r="134" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A134" s="1">
         <v>44865</v>
       </c>
@@ -12458,7 +12465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:28">
+    <row r="135" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A135" s="1">
         <v>44866</v>
       </c>
@@ -12544,7 +12551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:28">
+    <row r="136" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A136" s="1">
         <v>44867</v>
       </c>
@@ -12627,6 +12634,178 @@
         <v>0</v>
       </c>
       <c r="AB136">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A137" s="1">
+        <v>44867</v>
+      </c>
+      <c r="B137" t="s">
+        <v>169</v>
+      </c>
+      <c r="C137" t="s">
+        <v>168</v>
+      </c>
+      <c r="D137">
+        <v>0</v>
+      </c>
+      <c r="E137">
+        <v>20</v>
+      </c>
+      <c r="F137">
+        <v>32.901000000000003</v>
+      </c>
+      <c r="G137">
+        <v>1</v>
+      </c>
+      <c r="H137">
+        <v>0</v>
+      </c>
+      <c r="I137">
+        <v>1</v>
+      </c>
+      <c r="J137">
+        <v>1</v>
+      </c>
+      <c r="K137">
+        <v>0</v>
+      </c>
+      <c r="L137">
+        <v>1</v>
+      </c>
+      <c r="M137">
+        <v>0</v>
+      </c>
+      <c r="N137">
+        <v>0</v>
+      </c>
+      <c r="O137">
+        <v>0</v>
+      </c>
+      <c r="P137">
+        <v>0</v>
+      </c>
+      <c r="Q137">
+        <v>0</v>
+      </c>
+      <c r="R137">
+        <v>0</v>
+      </c>
+      <c r="S137">
+        <v>0</v>
+      </c>
+      <c r="T137">
+        <v>0</v>
+      </c>
+      <c r="U137">
+        <v>0</v>
+      </c>
+      <c r="V137">
+        <v>0</v>
+      </c>
+      <c r="W137">
+        <v>0</v>
+      </c>
+      <c r="X137">
+        <v>0</v>
+      </c>
+      <c r="Y137">
+        <v>0</v>
+      </c>
+      <c r="Z137">
+        <v>0</v>
+      </c>
+      <c r="AA137">
+        <v>0</v>
+      </c>
+      <c r="AB137">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+      <c r="A138" s="1">
+        <v>44867</v>
+      </c>
+      <c r="B138" t="s">
+        <v>167</v>
+      </c>
+      <c r="C138" t="s">
+        <v>47</v>
+      </c>
+      <c r="D138">
+        <v>0</v>
+      </c>
+      <c r="E138">
+        <v>60</v>
+      </c>
+      <c r="F138">
+        <v>15.31</v>
+      </c>
+      <c r="G138">
+        <v>1</v>
+      </c>
+      <c r="H138">
+        <v>0</v>
+      </c>
+      <c r="I138">
+        <v>1</v>
+      </c>
+      <c r="J138">
+        <v>0</v>
+      </c>
+      <c r="K138">
+        <v>0</v>
+      </c>
+      <c r="L138">
+        <v>0</v>
+      </c>
+      <c r="M138">
+        <v>0</v>
+      </c>
+      <c r="N138">
+        <v>1</v>
+      </c>
+      <c r="O138">
+        <v>1</v>
+      </c>
+      <c r="P138">
+        <v>1</v>
+      </c>
+      <c r="Q138">
+        <v>0</v>
+      </c>
+      <c r="R138">
+        <v>1</v>
+      </c>
+      <c r="S138">
+        <v>0</v>
+      </c>
+      <c r="T138">
+        <v>0</v>
+      </c>
+      <c r="U138">
+        <v>1</v>
+      </c>
+      <c r="V138">
+        <v>0</v>
+      </c>
+      <c r="W138">
+        <v>0</v>
+      </c>
+      <c r="X138">
+        <v>0</v>
+      </c>
+      <c r="Y138">
+        <v>1</v>
+      </c>
+      <c r="Z138">
+        <v>0</v>
+      </c>
+      <c r="AA138">
+        <v>0</v>
+      </c>
+      <c r="AB138">
         <v>0</v>
       </c>
     </row>

</xml_diff>